<commit_message>
Now handles empty Balancing Segment
</commit_message>
<xml_diff>
--- a/excel-data-files/currrency-translate-gl-account-balances-ggp.xlsx
+++ b/excel-data-files/currrency-translate-gl-account-balances-ggp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardguy/r/oracleplaywright/excel-data-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64E34E0-8148-7C48-9A7D-CA20626DCC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668866FA-762F-7344-8938-AF2C4B911706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17860" yWindow="760" windowWidth="16700" windowHeight="21580" activeTab="2" xr2:uid="{39C55B49-5ADB-CF4F-8459-6E15E59B12DD}"/>
+    <workbookView xWindow="3000" yWindow="-19180" windowWidth="22060" windowHeight="13760" activeTab="2" xr2:uid="{39C55B49-5ADB-CF4F-8459-6E15E59B12DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Loop-MG" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Loop!$B$1:$E$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Loop!$B$1:$E$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Loop-all'!$B$1:$E$640</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3161" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3144" uniqueCount="382">
   <si>
     <t>url</t>
   </si>
@@ -1702,7 +1702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B25D91-67B5-EF48-9DB9-A33972D99E99}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1762,17 +1762,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C954161-31AF-7544-AE12-35891B6760E8}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1812,36 +1813,36 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
-        <v>270000</v>
+      <c r="E3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
-        <v>270000</v>
+      <c r="E4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1849,16 +1850,16 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>381</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1872,10 +1873,7 @@
         <v>381</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1883,16 +1881,13 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>381</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1906,70 +1901,11 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>381</v>
-      </c>
-      <c r="D9" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>381</v>
-      </c>
-      <c r="D10" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>380</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:E12" xr:uid="{B6BF1AF1-BB48-BE41-A69F-F47EDEE8F8CA}"/>
+  <autoFilter ref="B1:E8" xr:uid="{B6BF1AF1-BB48-BE41-A69F-F47EDEE8F8CA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>